<commit_message>
- update RE scripts names - small fixes in fama 1970 apps
</commit_message>
<xml_diff>
--- a/revue_economique/data/metatopics.xlsx
+++ b/revue_economique/data/metatopics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\MEGA\data\revue_economique_project\intermediate_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cloud\research\revue_economique\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BF8280-F222-4F3B-9CE6-12F7AFD29546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973FEEB9-1B4A-4D3D-A294-A5D2497AAC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="3" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>Gestion du risque et prévention</t>
   </si>
   <si>
-    <t>Néo-institutionalisme et conventions</t>
-  </si>
-  <si>
     <t>Réglementation des marchés</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>Production / capital</t>
+  </si>
+  <si>
+    <t>Néo-institutionnalisme et conventions</t>
   </si>
 </sst>
 </file>
@@ -530,16 +530,16 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,29 +553,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>11</v>
       </c>
@@ -586,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>12</v>
       </c>
@@ -597,7 +597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>15</v>
       </c>
@@ -608,7 +608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>24</v>
       </c>
@@ -619,7 +619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -630,7 +630,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>19</v>
       </c>
@@ -644,12 +644,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>29</v>
@@ -658,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2</v>
       </c>
@@ -669,7 +669,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -680,18 +680,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>17</v>
       </c>
@@ -702,29 +702,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>8</v>
       </c>
@@ -735,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>28</v>
       </c>
@@ -746,7 +746,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -757,7 +757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -771,7 +771,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>14</v>
       </c>
@@ -782,19 +782,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -808,18 +808,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>29</v>
       </c>
@@ -833,7 +833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>13</v>
       </c>
@@ -844,7 +844,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>3</v>
       </c>
@@ -855,7 +855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>9</v>
       </c>
@@ -867,7 +867,7 @@
       </c>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>22</v>
       </c>
@@ -878,18 +878,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>26</v>
       </c>

</xml_diff>